<commit_message>
Add new Excel template for school list and enhance report parsing functionality
- Introduced a new Excel template for 'Danh sách trường đã gửi' to support school list reporting.
- Updated options to include the new template in the report selection.
- Improved report parsing logic to handle school data more effectively, including sorting and formatting.
- Refactored utility functions to integrate school names and ward information from the cities data.
</commit_message>
<xml_diff>
--- a/public/templates/truong_lop_hs.xlsx
+++ b/public/templates/truong_lop_hs.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\survey-form\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4117BF64-EE4F-4ADB-A2F3-7A90AAF6D2AC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24E0DED7-4E64-41CA-B243-217301904238}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12105" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -140,7 +140,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -152,7 +152,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -496,7 +495,7 @@
   <dimension ref="B3:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -532,7 +531,7 @@
         <f>SUM(D5:D9)</f>
         <v>0</v>
       </c>
-      <c r="E4" s="10">
+      <c r="E4" s="9">
         <f>C4-D4</f>
         <v>1605</v>
       </c>
@@ -544,7 +543,7 @@
       <c r="C5" s="2">
         <v>527</v>
       </c>
-      <c r="D5" s="1"/>
+      <c r="D5" s="8"/>
       <c r="E5" s="8">
         <f t="shared" ref="E5:E21" si="0">C5-D5</f>
         <v>527</v>
@@ -557,7 +556,7 @@
       <c r="C6" s="2">
         <v>564</v>
       </c>
-      <c r="D6" s="1"/>
+      <c r="D6" s="8"/>
       <c r="E6" s="8">
         <f t="shared" si="0"/>
         <v>564</v>
@@ -570,7 +569,7 @@
       <c r="C7" s="2">
         <v>365</v>
       </c>
-      <c r="D7" s="1"/>
+      <c r="D7" s="8"/>
       <c r="E7" s="8">
         <f t="shared" si="0"/>
         <v>365</v>
@@ -583,7 +582,7 @@
       <c r="C8" s="2">
         <v>122</v>
       </c>
-      <c r="D8" s="1"/>
+      <c r="D8" s="8"/>
       <c r="E8" s="8">
         <f t="shared" si="0"/>
         <v>122</v>
@@ -596,7 +595,7 @@
       <c r="C9" s="2">
         <v>27</v>
       </c>
-      <c r="D9" s="1"/>
+      <c r="D9" s="8"/>
       <c r="E9" s="8">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -609,11 +608,11 @@
       <c r="C10" s="4">
         <v>37459</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10" s="9">
         <f>SUM(D11:D15)</f>
         <v>0</v>
       </c>
-      <c r="E10" s="10">
+      <c r="E10" s="9">
         <f t="shared" si="0"/>
         <v>37459</v>
       </c>
@@ -625,7 +624,7 @@
       <c r="C11" s="2">
         <v>7231</v>
       </c>
-      <c r="D11" s="1"/>
+      <c r="D11" s="8"/>
       <c r="E11" s="8">
         <f t="shared" si="0"/>
         <v>7231</v>
@@ -638,7 +637,7 @@
       <c r="C12" s="2">
         <v>13491</v>
       </c>
-      <c r="D12" s="1"/>
+      <c r="D12" s="8"/>
       <c r="E12" s="8">
         <f t="shared" si="0"/>
         <v>13491</v>
@@ -651,7 +650,7 @@
       <c r="C13" s="2">
         <v>10164</v>
       </c>
-      <c r="D13" s="1"/>
+      <c r="D13" s="8"/>
       <c r="E13" s="8">
         <f t="shared" si="0"/>
         <v>10164</v>
@@ -664,7 +663,7 @@
       <c r="C14" s="2">
         <v>6317</v>
       </c>
-      <c r="D14" s="1"/>
+      <c r="D14" s="8"/>
       <c r="E14" s="8">
         <f t="shared" si="0"/>
         <v>6317</v>
@@ -677,7 +676,7 @@
       <c r="C15" s="2">
         <v>256</v>
       </c>
-      <c r="D15" s="1"/>
+      <c r="D15" s="8"/>
       <c r="E15" s="8">
         <f t="shared" si="0"/>
         <v>256</v>
@@ -690,11 +689,11 @@
       <c r="C16" s="4">
         <v>808873</v>
       </c>
-      <c r="D16" s="3">
+      <c r="D16" s="9">
         <f>SUM(D17:D21)</f>
         <v>0</v>
       </c>
-      <c r="E16" s="10">
+      <c r="E16" s="9">
         <f t="shared" si="0"/>
         <v>808873</v>
       </c>
@@ -706,7 +705,7 @@
       <c r="C17" s="2">
         <v>117925</v>
       </c>
-      <c r="D17" s="1"/>
+      <c r="D17" s="8"/>
       <c r="E17" s="8">
         <f t="shared" si="0"/>
         <v>117925</v>
@@ -719,7 +718,7 @@
       <c r="C18" s="2">
         <v>322382</v>
       </c>
-      <c r="D18" s="1"/>
+      <c r="D18" s="8"/>
       <c r="E18" s="8">
         <f t="shared" si="0"/>
         <v>322382</v>
@@ -732,7 +731,7 @@
       <c r="C19" s="2">
         <v>243173</v>
       </c>
-      <c r="D19" s="1"/>
+      <c r="D19" s="8"/>
       <c r="E19" s="8">
         <f t="shared" si="0"/>
         <v>243173</v>
@@ -745,7 +744,7 @@
       <c r="C20" s="2">
         <v>120809</v>
       </c>
-      <c r="D20" s="1"/>
+      <c r="D20" s="8"/>
       <c r="E20" s="8">
         <f t="shared" si="0"/>
         <v>120809</v>
@@ -758,7 +757,7 @@
       <c r="C21" s="2">
         <v>4584</v>
       </c>
-      <c r="D21" s="1"/>
+      <c r="D21" s="8"/>
       <c r="E21" s="8">
         <f t="shared" si="0"/>
         <v>4584</v>
@@ -766,6 +765,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>